<commit_message>
SolicitudGrafica_CN_08_06_REC30 y corrección de códigos
Nueva solicitud, y se corrigen los códigos de las demás, pues aparecía
como 08_01 y no 08_06. Las imágenes no cambian.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion06/SolicitudGrafica_CN_08_06_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion06/SolicitudGrafica_CN_08_06_CO.xlsx
@@ -508,9 +508,6 @@
     <t>Miguel Aljure</t>
   </si>
   <si>
-    <t>CN_08_01_CO_REC10</t>
-  </si>
-  <si>
     <t>Fundamentos de genética</t>
   </si>
   <si>
@@ -647,6 +644,9 @@
   </si>
   <si>
     <t>157769456 y https://commons.wikimedia.org/wiki/File:Gregor_Mendel_Monk.jpg</t>
+  </si>
+  <si>
+    <t>CN_08_06_CO</t>
   </si>
 </sst>
 </file>
@@ -1622,6 +1622,22 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="51" applyFont="1"/>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1705,22 +1721,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="51" applyFont="1"/>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -2672,7 +2672,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2710,14 +2710,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="F2" s="89" t="s">
+      <c r="D2" s="103"/>
+      <c r="F2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="90"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
       <c r="J2" s="16"/>
@@ -2727,14 +2727,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="98">
+      <c r="C3" s="104">
         <v>8</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="F3" s="91">
+      <c r="D3" s="105"/>
+      <c r="F3" s="97">
         <v>42131</v>
       </c>
-      <c r="G3" s="92"/>
+      <c r="G3" s="98"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
       <c r="J3" s="16"/>
@@ -2744,16 +2744,16 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="98" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="99"/>
+      <c r="C4" s="104" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="105"/>
       <c r="E4" s="5"/>
       <c r="F4" s="50" t="s">
         <v>55</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H4" s="51"/>
       <c r="I4" s="51"/>
@@ -2765,10 +2765,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="101"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="5"/>
       <c r="F5" s="48" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2799,7 +2799,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>39</v>
@@ -2817,12 +2817,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="93" t="s">
+      <c r="F8" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="95"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="101"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2872,21 +2872,21 @@
         <v>IMG01</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" s="27" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_01_CO_REC10_IMG01_small</v>
+        <v>CN_08_06_CO_IMG01_small</v>
       </c>
       <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2894,14 +2894,14 @@
       </c>
       <c r="H10" s="14" t="str">
         <f>IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_08_01_CO_REC10_IMG01_zoom</v>
+        <v>CN_08_06_CO_IMG01_zoom</v>
       </c>
       <c r="I10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="19"/>
     </row>
@@ -2918,14 +2918,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F74" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_01_CO_REC10_IMG02_small</v>
+        <v>CN_08_06_CO_IMG02_small</v>
       </c>
       <c r="G11" s="14" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2933,56 +2933,56 @@
       </c>
       <c r="H11" s="14" t="str">
         <f t="shared" ref="H11:H74" si="2">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_08_01_CO_REC10_IMG02_zoom</v>
+        <v>CN_08_06_CO_IMG02_zoom</v>
       </c>
       <c r="I11" s="14" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="1:16" s="125" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A12" s="120" t="str">
+    <row r="12" spans="1:16" s="94" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="89" t="str">
         <f t="shared" ref="A12:A30" si="3">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="121" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" s="122" t="str">
+      <c r="B12" s="90" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="91" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D12" s="123" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12" s="123" t="s">
-        <v>151</v>
-      </c>
-      <c r="F12" s="123" t="str">
+      <c r="D12" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="92" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="92" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG03_small</v>
-      </c>
-      <c r="G12" s="123" t="str">
+        <v>CN_08_06_CO_IMG03_small</v>
+      </c>
+      <c r="G12" s="92" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H12" s="123" t="str">
+      <c r="H12" s="92" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG03_zoom</v>
-      </c>
-      <c r="I12" s="123" t="str">
+        <v>CN_08_06_CO_IMG03_zoom</v>
+      </c>
+      <c r="I12" s="92" t="str">
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="124" t="s">
+      <c r="J12" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="K12" s="93" t="s">
         <v>154</v>
-      </c>
-      <c r="K12" s="124" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -2998,14 +2998,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG04_small</v>
+        <v>CN_08_06_CO_IMG04_small</v>
       </c>
       <c r="G13" s="14" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3013,17 +3013,17 @@
       </c>
       <c r="H13" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG04_zoom</v>
+        <v>CN_08_06_CO_IMG04_zoom</v>
       </c>
       <c r="I13" s="14" t="str">
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="K13" s="79" t="s">
         <v>157</v>
-      </c>
-      <c r="K13" s="79" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -3032,21 +3032,21 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG05_small</v>
+        <v>CN_08_06_CO_IMG05_small</v>
       </c>
       <c r="G14" s="14" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3054,17 +3054,17 @@
       </c>
       <c r="H14" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG05_zoom</v>
+        <v>CN_08_06_CO_IMG05_zoom</v>
       </c>
       <c r="I14" s="14" t="str">
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="87" t="s">
+        <v>178</v>
+      </c>
+      <c r="K14" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="247.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3073,21 +3073,21 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG06_small</v>
+        <v>CN_08_06_CO_IMG06_small</v>
       </c>
       <c r="G15" s="14" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3095,17 +3095,17 @@
       </c>
       <c r="H15" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG06_zoom</v>
+        <v>CN_08_06_CO_IMG06_zoom</v>
       </c>
       <c r="I15" s="14" t="str">
         <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K15" s="82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
@@ -3121,14 +3121,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG07_small</v>
+        <v>CN_08_06_CO_IMG07_small</v>
       </c>
       <c r="G16" s="14" t="str">
         <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3136,17 +3136,17 @@
       </c>
       <c r="H16" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG07_zoom</v>
+        <v>CN_08_06_CO_IMG07_zoom</v>
       </c>
       <c r="I16" s="14" t="str">
         <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="K16" s="84" t="s">
         <v>162</v>
-      </c>
-      <c r="K16" s="84" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -3162,14 +3162,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F17" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG08_small</v>
+        <v>CN_08_06_CO_IMG08_small</v>
       </c>
       <c r="G17" s="14" t="str">
         <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3177,14 +3177,14 @@
       </c>
       <c r="H17" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG08_zoom</v>
+        <v>CN_08_06_CO_IMG08_zoom</v>
       </c>
       <c r="I17" s="14" t="str">
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K17" s="21"/>
     </row>
@@ -3201,14 +3201,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG09_small</v>
+        <v>CN_08_06_CO_IMG09_small</v>
       </c>
       <c r="G18" s="14" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3216,20 +3216,20 @@
       </c>
       <c r="H18" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG09_zoom</v>
+        <v>CN_08_06_CO_IMG09_zoom</v>
       </c>
       <c r="I18" s="14" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="82" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="171" x14ac:dyDescent="0.3">
       <c r="A19" s="85" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="80">
         <v>248376691</v>
@@ -3239,14 +3239,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F19" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG10_small</v>
+        <v>CN_08_06_CO_IMG10_small</v>
       </c>
       <c r="G19" s="14" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3254,39 +3254,39 @@
       </c>
       <c r="H19" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG10_zoom</v>
+        <v>CN_08_06_CO_IMG10_zoom</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="K19" s="84" t="s">
         <v>166</v>
-      </c>
-      <c r="K19" s="84" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A20" s="85" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B20" s="86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C20" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F20" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG11_small</v>
+        <v>CN_08_06_CO_IMG11_small</v>
       </c>
       <c r="G20" s="14" t="str">
         <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3294,20 +3294,20 @@
       </c>
       <c r="H20" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG11_zoom</v>
+        <v>CN_08_06_CO_IMG11_zoom</v>
       </c>
       <c r="I20" s="14" t="str">
         <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="77" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="85" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" s="78">
         <v>160388525</v>
@@ -3317,14 +3317,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F21" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG12_small</v>
+        <v>CN_08_06_CO_IMG12_small</v>
       </c>
       <c r="G21" s="14" t="str">
         <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3332,22 +3332,22 @@
       </c>
       <c r="H21" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG12_zoom</v>
+        <v>CN_08_06_CO_IMG12_zoom</v>
       </c>
       <c r="I21" s="14" t="str">
         <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K21" s="82" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A22" s="85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B22" s="87">
         <v>93013351</v>
@@ -3357,14 +3357,14 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>151</v>
       </c>
       <c r="F22" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG13_small</v>
+        <v>CN_08_06_CO_IMG13_small</v>
       </c>
       <c r="G22" s="14" t="str">
         <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3372,37 +3372,37 @@
       </c>
       <c r="H22" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG13_zoom</v>
+        <v>CN_08_06_CO_IMG13_zoom</v>
       </c>
       <c r="I22" s="14" t="str">
         <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="76" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:11" s="12" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="85" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" s="87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C23" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG14_small</v>
+        <v>CN_08_06_CO_IMG14_small</v>
       </c>
       <c r="G23" s="14" t="str">
         <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3410,39 +3410,39 @@
       </c>
       <c r="H23" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG14_zoom</v>
+        <v>CN_08_06_CO_IMG14_zoom</v>
       </c>
       <c r="I23" s="14" t="str">
         <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K23" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="85" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C24" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F24" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG15_small</v>
+        <v>CN_08_06_CO_IMG15_small</v>
       </c>
       <c r="G24" s="14" t="str">
         <f>IF(F24&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3450,39 +3450,39 @@
       </c>
       <c r="H24" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG15_zoom</v>
+        <v>CN_08_06_CO_IMG15_zoom</v>
       </c>
       <c r="I24" s="14" t="str">
         <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" ht="336" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="85" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" s="87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F25" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_08_01_CO_REC10_IMG16_small</v>
+        <v>CN_08_06_CO_IMG16_small</v>
       </c>
       <c r="G25" s="14" t="str">
         <f>IF(F25&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3490,17 +3490,17 @@
       </c>
       <c r="H25" s="14" t="str">
         <f t="shared" si="2"/>
-        <v>CN_08_01_CO_REC10_IMG16_zoom</v>
+        <v>CN_08_06_CO_IMG16_zoom</v>
       </c>
       <c r="I25" s="14" t="str">
         <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -5682,25 +5682,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="112"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="42"/>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="108"/>
-      <c r="E2" s="109"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="115"/>
       <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -5708,11 +5708,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="42"/>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="115"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="121"/>
       <c r="F3" s="43"/>
       <c r="H3" s="33" t="s">
         <v>18</v>
@@ -5763,11 +5763,11 @@
       <c r="C5" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="116" t="str">
+      <c r="D5" s="122" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="117"/>
+      <c r="E5" s="123"/>
       <c r="F5" s="43"/>
       <c r="H5" s="33" t="s">
         <v>22</v>
@@ -5812,12 +5812,12 @@
       <c r="C7" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="102" t="str">
+      <c r="D7" s="108" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="102"/>
-      <c r="F7" s="103"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="109"/>
       <c r="H7" s="33" t="s">
         <v>24</v>
       </c>
@@ -5911,14 +5911,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="106"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="112"/>
       <c r="I13" s="33" t="s">
         <v>33</v>
       </c>
@@ -5951,12 +5951,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="42"/>
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="113" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="108"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="114"/>
+      <c r="F15" s="115"/>
       <c r="J15" s="33">
         <v>12</v>
       </c>
@@ -5996,12 +5996,12 @@
       <c r="C17" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="110" t="str">
+      <c r="D17" s="116" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="111"/>
-      <c r="F17" s="112"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="118"/>
       <c r="J17" s="33">
         <v>14</v>
       </c>
@@ -6017,12 +6017,12 @@
       <c r="C18" s="73" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="102" t="str">
+      <c r="D18" s="108" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="102"/>
-      <c r="F18" s="103"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="109"/>
       <c r="J18" s="33">
         <v>15</v>
       </c>
@@ -6414,41 +6414,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="118" t="s">
+      <c r="F1" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="119" t="s">
+      <c r="H1" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="A2" s="124"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
       <c r="H2" s="52" t="s">
         <v>65</v>
       </c>

</xml_diff>